<commit_message>
Added Flags testing script
</commit_message>
<xml_diff>
--- a/Naga V0/Control Microcode EEPROM Programmer/Scripts.xlsx
+++ b/Naga V0/Control Microcode EEPROM Programmer/Scripts.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronit\OneDrive\Desktop\8-bit-computer\Naga V0\Control Microcode EEPROM Programmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{22871671-636C-41CA-87E0-DEBB61617BBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5B45F8-BD80-474B-A782-8330ACC83CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2A5A9182-85BD-49DB-A3DB-4B4AEEB46DFD}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Loop Code" sheetId="2" r:id="rId1"/>
+    <sheet name="Flags Test" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="37">
   <si>
     <t>Memory Location</t>
   </si>
@@ -65,9 +66,6 @@
     <t>0b0001</t>
   </si>
   <si>
-    <t>LBI</t>
-  </si>
-  <si>
     <t>0b0010</t>
   </si>
   <si>
@@ -89,9 +87,6 @@
     <t>0b0101</t>
   </si>
   <si>
-    <t>INC</t>
-  </si>
-  <si>
     <t>0b0110</t>
   </si>
   <si>
@@ -116,13 +111,43 @@
     <t>0b1101</t>
   </si>
   <si>
-    <t>0b00000000</t>
-  </si>
-  <si>
-    <t>Current Val</t>
-  </si>
-  <si>
-    <t>Index</t>
+    <t>LDB</t>
+  </si>
+  <si>
+    <t>ADD</t>
+  </si>
+  <si>
+    <t>JC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OUT </t>
+  </si>
+  <si>
+    <t>HLT</t>
+  </si>
+  <si>
+    <t>Opcode</t>
+  </si>
+  <si>
+    <t>NOP</t>
+  </si>
+  <si>
+    <t>LDI</t>
+  </si>
+  <si>
+    <t>JMP</t>
+  </si>
+  <si>
+    <t>JZ</t>
+  </si>
+  <si>
+    <t>JN</t>
+  </si>
+  <si>
+    <t>OUT</t>
+  </si>
+  <si>
+    <t>"0110"</t>
   </si>
 </sst>
 </file>
@@ -476,16 +501,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21A549A-DA8E-4754-BE4C-E053EFDABF08}">
-  <dimension ref="A1:E17"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E14371EA-436F-4C96-884A-2FC294D0E6E7}">
+  <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:E17"/>
+      <selection activeCell="B16" sqref="B16:C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -501,138 +529,535 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+        <v>35</v>
+      </c>
+      <c r="C2">
+        <v>1110</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="str">
+        <f>RIGHT(A2, 4)</f>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>8</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>1111</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I17" si="0">RIGHT(A3, 4)</f>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
         <v>9</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>0010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5">
+        <v>1110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>0011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>0100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>32</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>0101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
         <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>12</v>
-      </c>
-      <c r="B5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C7" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>18</v>
-      </c>
-      <c r="B8" t="s">
-        <v>13</v>
       </c>
       <c r="C8">
         <v>1111</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>0110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9">
+        <v>1110</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>0111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" t="s">
+        <v>35</v>
+      </c>
+      <c r="C10">
+        <v>1110</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+      <c r="B11" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+      <c r="C12">
+        <v>110</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>7</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="1">
+        <v>0</v>
+      </c>
+      <c r="C16" s="1"/>
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>1</v>
+      </c>
+      <c r="C17" s="1"/>
+      <c r="H17" t="s">
+        <v>28</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B17:C17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D21A549A-DA8E-4754-BE4C-E053EFDABF08}">
+  <dimension ref="A1:I17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D28" sqref="D28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="4" max="4" width="11" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2">
+        <v>1110</v>
+      </c>
+      <c r="E2" t="str">
+        <f>LOOKUP(B2, H2:I17)</f>
+        <v>1010</v>
+      </c>
+      <c r="H2" t="s">
+        <v>30</v>
+      </c>
+      <c r="I2" t="str">
+        <f>RIGHT(A2, 4)</f>
+        <v>0000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3">
+        <v>1111</v>
+      </c>
+      <c r="H3" t="s">
+        <v>6</v>
+      </c>
+      <c r="I3" t="str">
+        <f t="shared" ref="I3:I17" si="0">RIGHT(A3, 4)</f>
+        <v>0001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" t="s">
+        <v>25</v>
+      </c>
+      <c r="H4" t="s">
+        <v>24</v>
+      </c>
+      <c r="I4" t="str">
+        <f t="shared" si="0"/>
+        <v>0010</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>26</v>
       </c>
+      <c r="C5">
+        <v>110</v>
+      </c>
+      <c r="H5" t="s">
+        <v>25</v>
+      </c>
+      <c r="I5" t="str">
+        <f t="shared" si="0"/>
+        <v>0011</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6">
+        <v>1101</v>
+      </c>
+      <c r="H6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" t="str">
+        <f t="shared" si="0"/>
+        <v>0100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7">
+        <v>1101</v>
+      </c>
+      <c r="H7" t="s">
+        <v>12</v>
+      </c>
+      <c r="I7" t="str">
+        <f t="shared" si="0"/>
+        <v>0101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" t="str">
+        <f t="shared" si="0"/>
+        <v>0110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="H9" t="s">
+        <v>32</v>
+      </c>
+      <c r="I9" t="str">
+        <f t="shared" si="0"/>
+        <v>0111</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="H10" t="s">
+        <v>33</v>
+      </c>
+      <c r="I10" t="str">
+        <f t="shared" si="0"/>
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="H11" t="s">
+        <v>34</v>
+      </c>
+      <c r="I11" t="str">
+        <f t="shared" si="0"/>
+        <v>1001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="H12" t="s">
+        <v>26</v>
+      </c>
+      <c r="I12" t="str">
+        <f t="shared" si="0"/>
+        <v>1010</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" t="str">
+        <f t="shared" si="0"/>
+        <v>1011</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>22</v>
+      </c>
+      <c r="I14" t="str">
+        <f t="shared" si="0"/>
+        <v>1100</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>23</v>
+      </c>
+      <c r="I15" t="str">
+        <f t="shared" si="0"/>
+        <v>1101</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>7</v>
+      </c>
+      <c r="B16" s="1">
+        <v>11000101</v>
+      </c>
       <c r="C16" s="1"/>
-      <c r="D16" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="H16" t="s">
+        <v>35</v>
+      </c>
+      <c r="I16" t="str">
+        <f t="shared" si="0"/>
+        <v>1110</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>26</v>
+        <v>14</v>
+      </c>
+      <c r="B17" s="1">
+        <v>10010110</v>
       </c>
       <c r="C17" s="1"/>
-      <c r="D17" t="s">
+      <c r="H17" t="s">
         <v>28</v>
+      </c>
+      <c r="I17" t="str">
+        <f t="shared" si="0"/>
+        <v>1111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized Loop Code LDB once
</commit_message>
<xml_diff>
--- a/Naga V0/Control Microcode EEPROM Programmer/Scripts.xlsx
+++ b/Naga V0/Control Microcode EEPROM Programmer/Scripts.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ronit\OneDrive\Desktop\8-bit-computer\Naga V0\Control Microcode EEPROM Programmer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F5B45F8-BD80-474B-A782-8330ACC83CC3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E09A5B5-C0F9-4D9C-AB5F-8453F2E82B60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{2A5A9182-85BD-49DB-A3DB-4B4AEEB46DFD}"/>
   </bookViews>
@@ -505,7 +505,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16:C16"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -538,10 +538,10 @@
         <v>5</v>
       </c>
       <c r="B2" t="s">
-        <v>35</v>
+        <v>24</v>
       </c>
       <c r="C2">
-        <v>1110</v>
+        <v>1111</v>
       </c>
       <c r="H2" t="s">
         <v>30</v>
@@ -556,10 +556,10 @@
         <v>8</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="C3">
-        <v>1111</v>
+        <v>1110</v>
       </c>
       <c r="H3" t="s">
         <v>6</v>
@@ -628,7 +628,7 @@
         <v>32</v>
       </c>
       <c r="C7">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H7" t="s">
         <v>12</v>
@@ -700,7 +700,7 @@
         <v>33</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H11" t="s">
         <v>34</v>

</xml_diff>